<commit_message>
Updated dt RRTMG code with diagnostics
</commit_message>
<xml_diff>
--- a/reduced_data/model_global_radiation_outputs.xlsx
+++ b/reduced_data/model_global_radiation_outputs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\University\University\MSc\Models\climate-analysis\reduced_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286AFDAF-5AF2-475E-A8D4-4CF3593259D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF4C6ED-189B-4014-A2AD-D812D7EC7394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4380" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34125" yWindow="-2565" windowWidth="21720" windowHeight="13830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>Model</t>
   </si>
@@ -121,6 +122,82 @@
   </si>
   <si>
     <t>best for ensemble</t>
+  </si>
+  <si>
+    <t>Model Output</t>
+  </si>
+  <si>
+    <t>4-year time integrated with absorber and model insolation inputs</t>
+  </si>
+  <si>
+    <t>CESM2-CAM6 (2007 to 2010)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4-year time integrated model with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT code absorber and insolation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4-year time integrated model with insolation inputs and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT code absorber</t>
+    </r>
+  </si>
+  <si>
+    <t>4-year mean model input with absorber and model insolation inputs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4-year mean model input with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT code absorber and insolation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4-year mean model input with insolation inputs and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEFAULT code absorber</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -150,15 +227,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,11 +249,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +289,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +585,13 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1099,16 +1222,231 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D1FB75-F9F2-4730-8DA7-E56DCF40304A}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5">
+        <v>50.171970000000002</v>
+      </c>
+      <c r="C2" s="5">
+        <v>247.09817000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>262.99484999999999</v>
+      </c>
+      <c r="E2" s="5">
+        <v>321.18352599999997</v>
+      </c>
+      <c r="F2" s="5">
+        <v>98.555750000000003</v>
+      </c>
+      <c r="G2" s="5">
+        <v>239.06726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10">
+        <v>59.640263330841996</v>
+      </c>
+      <c r="C3" s="10">
+        <v>221.75372661544699</v>
+      </c>
+      <c r="D3" s="10">
+        <v>258.73008899669702</v>
+      </c>
+      <c r="E3" s="10">
+        <v>314.61171440793697</v>
+      </c>
+      <c r="F3" s="10">
+        <v>91.236324329381205</v>
+      </c>
+      <c r="G3" s="10">
+        <v>244.12810098399001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="10">
+        <v>59.429717135418102</v>
+      </c>
+      <c r="C4" s="10">
+        <v>221.45308833320999</v>
+      </c>
+      <c r="D4" s="10">
+        <v>259.898643652072</v>
+      </c>
+      <c r="E4" s="10">
+        <v>313.57883490079797</v>
+      </c>
+      <c r="F4" s="10">
+        <v>90.952710666854301</v>
+      </c>
+      <c r="G4" s="10">
+        <v>245.11551248174601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="10">
+        <v>69.249927388614495</v>
+      </c>
+      <c r="C5" s="10">
+        <v>219.566140646642</v>
+      </c>
+      <c r="D5" s="10">
+        <v>259.898643652072</v>
+      </c>
+      <c r="E5" s="10">
+        <v>313.57883490079797</v>
+      </c>
+      <c r="F5" s="10">
+        <v>105.563347451116</v>
+      </c>
+      <c r="G5" s="10">
+        <v>245.11551248174601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="10">
+        <v>60.895812051407397</v>
+      </c>
+      <c r="C7" s="10">
+        <v>219.06610982484401</v>
+      </c>
+      <c r="D7" s="10">
+        <v>257.86295284807801</v>
+      </c>
+      <c r="E7" s="10">
+        <v>314.50510784473499</v>
+      </c>
+      <c r="F7" s="10">
+        <v>93.497087356956001</v>
+      </c>
+      <c r="G7" s="10">
+        <v>244.052031294931</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="10">
+        <v>60.666068955977899</v>
+      </c>
+      <c r="C8" s="10">
+        <v>218.74313984464601</v>
+      </c>
+      <c r="D8" s="10">
+        <v>259.05352555273902</v>
+      </c>
+      <c r="E8" s="10">
+        <v>313.48475757092899</v>
+      </c>
+      <c r="F8" s="10">
+        <v>93.190002362781996</v>
+      </c>
+      <c r="G8" s="10">
+        <v>245.07313321087199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="10">
+        <v>66.692594425501497</v>
+      </c>
+      <c r="C9" s="10">
+        <v>218.94504449832101</v>
+      </c>
+      <c r="D9" s="10">
+        <v>259.05352555273902</v>
+      </c>
+      <c r="E9" s="10">
+        <v>313.48475757092899</v>
+      </c>
+      <c r="F9" s="10">
+        <v>102.749234023854</v>
+      </c>
+      <c r="G9" s="10">
+        <v>245.07313321087199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF242D4-48AF-4D8F-926F-D433A993891A}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>